<commit_message>
Oppdater felter-faner i test-kodebok
</commit_message>
<xml_diff>
--- a/tests/testthat/testdata/mrs5-kodebok/parse_kodebok_feil_skjema.xlsx
+++ b/tests/testthat/testdata/mrs5-kodebok/parse_kodebok_feil_skjema.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\endevj\OneDrive - Helse Vest\rapwhale\tests\testthat\testdata\mrs5-kodebok\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59563245-3F3D-4289-83D2-2A7E820682D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDF45E96-1096-462E-A7CB-3A89354E05A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{532BB522-EB7E-4931-B041-1D7FE65AB65E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="5" xr2:uid="{532BB522-EB7E-4931-B041-1D7FE65AB65E}"/>
   </bookViews>
   <sheets>
     <sheet name="Generelt" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="53">
   <si>
     <t>Skjematypenavn</t>
   </si>
@@ -621,8 +621,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DBBD1B60-3C2A-4299-AB00-41349CF58D2B}">
   <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -942,12 +942,283 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA42ACE6-2FE8-4E7C-A1D8-88580F11CF75}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Følsomhet Intern (gul)</oddFooter>
@@ -1252,12 +1523,283 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D9C3C218-1E63-4B7E-8D0F-E4852BC2068E}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="A12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="1"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter>&amp;L_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Følsomhet Intern (gul)</oddFooter>

</xml_diff>